<commit_message>
mac Vin 15 Iul 2022 10:05:24 EEST
</commit_message>
<xml_diff>
--- a/SCRATCH/RELEASE/foaie_parcurs_B-151-VGT_iunie_2022_Alex_Bora.xlsx
+++ b/SCRATCH/RELEASE/foaie_parcurs_B-151-VGT_iunie_2022_Alex_Bora.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="38">
   <si>
     <t>VOLVO ROMÂNIA</t>
   </si>
@@ -70,42 +70,45 @@
     <t>Observatii utilizator</t>
   </si>
   <si>
+    <t>Acasa-Birou</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Cluj-Bontida</t>
+  </si>
+  <si>
+    <t>Interes Serviciu</t>
+  </si>
+  <si>
+    <t>Cluj-Satu-Mare</t>
+  </si>
+  <si>
+    <t>Cluj-Bistrita</t>
+  </si>
+  <si>
+    <t>Cluj-Dej</t>
+  </si>
+  <si>
+    <t>Cluj-Baia-Mare</t>
+  </si>
+  <si>
+    <t>Cluj-Cluj</t>
+  </si>
+  <si>
+    <t>Cluj-Apahida</t>
+  </si>
+  <si>
+    <t>Cluj-Zalau</t>
+  </si>
+  <si>
+    <t>Cluj-Cmp. Turzii</t>
+  </si>
+  <si>
     <t>Cluj-Turda</t>
   </si>
   <si>
-    <t>Interes Serviciu</t>
-  </si>
-  <si>
-    <t>Cluj-Satu-Mare</t>
-  </si>
-  <si>
-    <t>Cluj-Apahida</t>
-  </si>
-  <si>
-    <t>Acasa-Birou</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>Cluj-Dej</t>
-  </si>
-  <si>
-    <t>Cluj-Cluj</t>
-  </si>
-  <si>
-    <t>Cluj-Baia-Mare</t>
-  </si>
-  <si>
-    <t>Cluj-Bontida</t>
-  </si>
-  <si>
-    <t>Cluj-Zalau</t>
-  </si>
-  <si>
-    <t>Cluj-Bistrita</t>
-  </si>
-  <si>
     <t>Km parcursi:</t>
   </si>
   <si>
@@ -124,7 +127,7 @@
     <t>Total km Personal Ratio		 0,0%</t>
   </si>
   <si>
-    <t>Semnătură utilizator:			  Data predarii: 01.06.2022</t>
+    <t>Semnătură utilizator:			  Data predarii: 01.07.2022</t>
   </si>
   <si>
     <t>……………………………………………………</t>
@@ -629,7 +632,7 @@
         <v>12</v>
       </c>
       <c r="B12" s="2">
-        <v>32742</v>
+        <v>43773</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="20" customHeight="1">
@@ -661,7 +664,7 @@
         <v>2</v>
       </c>
       <c r="B15" s="4">
-        <v>121</v>
+        <v>30</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>17</v>
@@ -675,10 +678,10 @@
         <v>3</v>
       </c>
       <c r="B16" s="4">
-        <v>421</v>
+        <v>30</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>18</v>
@@ -709,13 +712,13 @@
         <v>6</v>
       </c>
       <c r="B19" s="4">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="20" customHeight="1">
@@ -726,10 +729,10 @@
         <v>30</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="20" customHeight="1">
@@ -737,13 +740,13 @@
         <v>8</v>
       </c>
       <c r="B21" s="4">
-        <v>101</v>
+        <v>421</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="20" customHeight="1">
@@ -751,13 +754,13 @@
         <v>9</v>
       </c>
       <c r="B22" s="4">
-        <v>47</v>
+        <v>257</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="20" customHeight="1">
@@ -765,10 +768,10 @@
         <v>10</v>
       </c>
       <c r="B23" s="4">
-        <v>356</v>
+        <v>30</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>18</v>
@@ -809,13 +812,13 @@
         <v>14</v>
       </c>
       <c r="B27" s="4">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="20" customHeight="1">
@@ -826,10 +829,10 @@
         <v>356</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="20" customHeight="1">
@@ -843,7 +846,7 @@
         <v>23</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="20" customHeight="1">
@@ -854,10 +857,10 @@
         <v>47</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="20" customHeight="1">
@@ -885,13 +888,13 @@
         <v>20</v>
       </c>
       <c r="B33" s="4">
-        <v>101</v>
+        <v>356</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="20" customHeight="1">
@@ -899,13 +902,13 @@
         <v>21</v>
       </c>
       <c r="B34" s="4">
-        <v>156</v>
+        <v>85</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="20" customHeight="1">
@@ -913,10 +916,10 @@
         <v>22</v>
       </c>
       <c r="B35" s="4">
-        <v>257</v>
+        <v>30</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="D35" s="4" t="s">
         <v>18</v>
@@ -927,13 +930,13 @@
         <v>23</v>
       </c>
       <c r="B36" s="4">
-        <v>30</v>
+        <v>156</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="20" customHeight="1">
@@ -941,10 +944,10 @@
         <v>24</v>
       </c>
       <c r="B37" s="4">
-        <v>257</v>
+        <v>30</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="D37" s="4" t="s">
         <v>18</v>
@@ -975,13 +978,13 @@
         <v>27</v>
       </c>
       <c r="B40" s="4">
-        <v>156</v>
+        <v>257</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="20" customHeight="1">
@@ -992,10 +995,10 @@
         <v>30</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="20" customHeight="1">
@@ -1003,13 +1006,13 @@
         <v>29</v>
       </c>
       <c r="B42" s="4">
-        <v>30</v>
+        <v>152</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="20" customHeight="1">
@@ -1020,56 +1023,56 @@
         <v>121</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="20" customHeight="1">
       <c r="A44" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B44" s="4">
-        <v>2895</v>
+        <v>2712</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="20" customHeight="1">
       <c r="A45" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B45" s="4">
-        <v>35637</v>
+        <v>46485</v>
       </c>
     </row>
     <row r="49" spans="1:1" ht="20" customHeight="1">
       <c r="A49" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="50" spans="1:1" ht="20" customHeight="1">
       <c r="A50" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="51" spans="1:1" ht="20" customHeight="1">
       <c r="A51" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="53" spans="1:1" ht="20" customHeight="1">
       <c r="A53" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="55" spans="1:1" ht="20" customHeight="1">
       <c r="A55" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="57" spans="1:1" ht="20" customHeight="1">
       <c r="A57" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feats - vineri 15 iulie 2022, 15:00:00 +0300
</commit_message>
<xml_diff>
--- a/SCRATCH/RELEASE/foaie_parcurs_B-151-VGT_iunie_2022_Alex_Bora.xlsx
+++ b/SCRATCH/RELEASE/foaie_parcurs_B-151-VGT_iunie_2022_Alex_Bora.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="37">
   <si>
     <t>VOLVO ROMÂNIA</t>
   </si>
@@ -70,43 +70,40 @@
     <t>Observatii utilizator</t>
   </si>
   <si>
+    <t>Cluj-Turda</t>
+  </si>
+  <si>
+    <t>Interes Serviciu</t>
+  </si>
+  <si>
+    <t>Cluj-Satu-Mare</t>
+  </si>
+  <si>
+    <t>Cluj-Apahida</t>
+  </si>
+  <si>
     <t>Acasa-Birou</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
+    <t>Cluj-Dej</t>
+  </si>
+  <si>
+    <t>Cluj-Cluj</t>
+  </si>
+  <si>
+    <t>Cluj-Baia-Mare</t>
+  </si>
+  <si>
     <t>Cluj-Bontida</t>
   </si>
   <si>
-    <t>Interes Serviciu</t>
-  </si>
-  <si>
-    <t>Cluj-Satu-Mare</t>
+    <t>Cluj-Zalau</t>
   </si>
   <si>
     <t>Cluj-Bistrita</t>
-  </si>
-  <si>
-    <t>Cluj-Dej</t>
-  </si>
-  <si>
-    <t>Cluj-Baia-Mare</t>
-  </si>
-  <si>
-    <t>Cluj-Cluj</t>
-  </si>
-  <si>
-    <t>Cluj-Apahida</t>
-  </si>
-  <si>
-    <t>Cluj-Zalau</t>
-  </si>
-  <si>
-    <t>Cluj-Cmp. Turzii</t>
-  </si>
-  <si>
-    <t>Cluj-Turda</t>
   </si>
   <si>
     <t>Km parcursi:</t>
@@ -632,7 +629,7 @@
         <v>12</v>
       </c>
       <c r="B12" s="2">
-        <v>43773</v>
+        <v>49380</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="20" customHeight="1">
@@ -664,7 +661,7 @@
         <v>2</v>
       </c>
       <c r="B15" s="4">
-        <v>30</v>
+        <v>121</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>17</v>
@@ -678,10 +675,10 @@
         <v>3</v>
       </c>
       <c r="B16" s="4">
-        <v>30</v>
+        <v>421</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>18</v>
@@ -712,13 +709,13 @@
         <v>6</v>
       </c>
       <c r="B19" s="4">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="20" customHeight="1">
@@ -729,10 +726,10 @@
         <v>30</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="20" customHeight="1">
@@ -740,13 +737,13 @@
         <v>8</v>
       </c>
       <c r="B21" s="4">
-        <v>421</v>
+        <v>101</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="20" customHeight="1">
@@ -754,13 +751,13 @@
         <v>9</v>
       </c>
       <c r="B22" s="4">
-        <v>257</v>
+        <v>47</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="20" customHeight="1">
@@ -768,10 +765,10 @@
         <v>10</v>
       </c>
       <c r="B23" s="4">
-        <v>30</v>
+        <v>356</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>18</v>
@@ -812,13 +809,13 @@
         <v>14</v>
       </c>
       <c r="B27" s="4">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="20" customHeight="1">
@@ -829,10 +826,10 @@
         <v>356</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="20" customHeight="1">
@@ -846,7 +843,7 @@
         <v>23</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="20" customHeight="1">
@@ -857,10 +854,10 @@
         <v>47</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="20" customHeight="1">
@@ -888,13 +885,13 @@
         <v>20</v>
       </c>
       <c r="B33" s="4">
-        <v>356</v>
+        <v>101</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="20" customHeight="1">
@@ -902,13 +899,13 @@
         <v>21</v>
       </c>
       <c r="B34" s="4">
-        <v>85</v>
+        <v>156</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="20" customHeight="1">
@@ -916,10 +913,10 @@
         <v>22</v>
       </c>
       <c r="B35" s="4">
-        <v>30</v>
+        <v>257</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="D35" s="4" t="s">
         <v>18</v>
@@ -930,13 +927,13 @@
         <v>23</v>
       </c>
       <c r="B36" s="4">
-        <v>156</v>
+        <v>30</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="20" customHeight="1">
@@ -944,10 +941,10 @@
         <v>24</v>
       </c>
       <c r="B37" s="4">
-        <v>30</v>
+        <v>257</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="D37" s="4" t="s">
         <v>18</v>
@@ -978,13 +975,13 @@
         <v>27</v>
       </c>
       <c r="B40" s="4">
-        <v>257</v>
+        <v>156</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="20" customHeight="1">
@@ -995,10 +992,10 @@
         <v>30</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="20" customHeight="1">
@@ -1006,13 +1003,13 @@
         <v>29</v>
       </c>
       <c r="B42" s="4">
-        <v>152</v>
+        <v>30</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="20" customHeight="1">
@@ -1023,56 +1020,56 @@
         <v>121</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="20" customHeight="1">
       <c r="A44" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B44" s="4">
-        <v>2712</v>
+        <v>2895</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="20" customHeight="1">
       <c r="A45" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B45" s="4">
-        <v>46485</v>
+        <v>52275</v>
       </c>
     </row>
     <row r="49" spans="1:1" ht="20" customHeight="1">
       <c r="A49" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="50" spans="1:1" ht="20" customHeight="1">
       <c r="A50" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="51" spans="1:1" ht="20" customHeight="1">
       <c r="A51" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="53" spans="1:1" ht="20" customHeight="1">
       <c r="A53" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="55" spans="1:1" ht="20" customHeight="1">
       <c r="A55" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="57" spans="1:1" ht="20" customHeight="1">
       <c r="A57" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>